<commit_message>
actualización de registros y no ignoramos la base de datos
</commit_message>
<xml_diff>
--- a/datos/Registros.xlsx
+++ b/datos/Registros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sino\Documents\MASTER PYTHON\TFM\Proyecto\OFO\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F6D25C-D208-4D69-93B7-ED56ED09AC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A5E0C4-42E2-4DFF-983C-31F1B7C65065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4801,7 +4801,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D325" sqref="D325"/>
+      <selection pane="bottomLeft" activeCell="H431" sqref="H431:H441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -63253,7 +63253,7 @@
       <c r="J1253" s="52"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="5">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N595:N620 K1011:N1242 N377:N585 N2:N374 K2:M585 K710:N711 K708:N708 K704:N704 K684:N686 K678:N680 K672:N673 N632 K662:N667 K652:N654 K644:N647 K595:M619 K586:N594" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$X$2:$X$3</formula1>
     </dataValidation>

</xml_diff>